<commit_message>
create DL SaoViet and DL TarisHN
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2021/Thang4/01.NhanBH/NBH210422_TarisHN.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2021/Thang4/01.NhanBH/NBH210422_TarisHN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhongBaoHanh\VNET\5. WS\1. Bộ phận bảo hành\1. Thực hiện sửa chữa bảo hành\nam2021\Thang4\01.NhanBH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VNET\5. WS\1. Bộ phận bảo hành\1. Thực hiện sửa chữa bảo hành\nam2021\Thang4\01.NhanBH\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t xml:space="preserve">STT </t>
   </si>
@@ -72,25 +72,31 @@
     <t>Ghi chú/Lô SX</t>
   </si>
   <si>
-    <t>Check lô sx đối với TG102LE/4G/E</t>
-  </si>
-  <si>
-    <t>ĐT :    +84915.22.33.99</t>
-  </si>
-  <si>
     <t>TG102LE</t>
   </si>
   <si>
-    <t>Hà Nội, ngày 14 tháng 04 Năm 2021</t>
-  </si>
-  <si>
-    <t>Tên cty/ cá nhân: VietCom</t>
-  </si>
-  <si>
-    <t>TG102E</t>
-  </si>
-  <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>Tên cty/ cá nhân: Taris Hà Nội</t>
+  </si>
+  <si>
+    <t>TG102V</t>
+  </si>
+  <si>
+    <t>TG102SE</t>
+  </si>
+  <si>
+    <t>Hà Nội, ngày 22 tháng 04 Năm 2021</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh Tùng</t>
+  </si>
+  <si>
+    <t>ĐT: 0915 22 33 99</t>
+  </si>
+  <si>
+    <t>Sim</t>
   </si>
 </sst>
 </file>
@@ -495,7 +501,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -514,9 +523,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -588,15 +594,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>23812</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>29765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1057275</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>1041797</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -619,8 +625,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1457325" cy="857250"/>
+          <a:off x="23812" y="29765"/>
+          <a:ext cx="1416844" cy="785812"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -919,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -932,7 +938,7 @@
     <col min="3" max="3" width="22.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="39" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -960,7 +966,7 @@
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="46" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
@@ -988,13 +994,13 @@
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
-      <c r="B6" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
+      <c r="B6" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
@@ -1008,23 +1014,23 @@
     </row>
     <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
@@ -1051,175 +1057,287 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="21">
-        <v>868183034634431</v>
-      </c>
-      <c r="D11" s="25"/>
+        <v>868183034681614</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="25"/>
+        <v>17</v>
+      </c>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="21">
-        <v>868183038050030</v>
-      </c>
-      <c r="D12" s="25"/>
+        <v>868183035868848</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="E12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="25"/>
+        <v>17</v>
+      </c>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>3</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" s="21">
-        <v>868183034584230</v>
-      </c>
-      <c r="D13" s="25"/>
+        <v>867717030424346</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="E13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="25"/>
+        <v>17</v>
+      </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="21">
+        <v>868183035913560</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="21">
+        <v>868183035926109</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="21">
+        <v>868183038519125</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="21">
+        <v>868183038069469</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="21">
+        <v>868345035586528</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="21">
+        <v>866192037845730</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="21">
+        <v>862631039238471</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="21">
-        <v>862549040720347</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="4" t="s">
+      <c r="E21" s="42"/>
+      <c r="F21" s="43"/>
+    </row>
+    <row r="22" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="D22" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27"/>
+    </row>
+    <row r="23" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="17"/>
+    </row>
+    <row r="25" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="25"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-    </row>
-    <row r="16" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
-    </row>
-    <row r="17" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-    </row>
-    <row r="22" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
-    </row>
-    <row r="23" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
+    </row>
+    <row r="28" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="20"/>
+    </row>
     <row r="29" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="8:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
+    <row r="34" spans="8:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="8:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="8:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="8:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="8:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="8:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D27:F27"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>